<commit_message>
added client table information for irwins
</commit_message>
<xml_diff>
--- a/documentation/Clients.xlsx
+++ b/documentation/Clients.xlsx
@@ -902,8 +902,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="d/mm/yyyy\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1401,8 +1401,8 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1730,7 +1730,7 @@
   <dimension ref="A1:FJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1739,16 @@
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="166" width="14.28515625" customWidth="1"/>
+    <col min="5" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="54" width="14.28515625" customWidth="1"/>
+    <col min="55" max="55" width="25.140625" customWidth="1"/>
+    <col min="56" max="125" width="14.28515625" customWidth="1"/>
+    <col min="126" max="126" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="22" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="19" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="49.42578125" customWidth="1"/>
+    <col min="130" max="166" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:166" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>